<commit_message>
Chore(UX) Update du jdt et du rapport.
</commit_message>
<xml_diff>
--- a/UX/jdt/JDT_OlayaMathis.xlsx
+++ b/UX/jdt/JDT_OlayaMathis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg24muu\Documents\GitHub\P_ShootMeUp\UX\jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B18283-4548-4442-91DB-F77F031D7C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C02C05-1F53-490E-B52A-AAD8CDCB54FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Auteur:</t>
   </si>
@@ -197,6 +197,12 @@
   </si>
   <si>
     <t>Je n'ai pas eu le temps de finir</t>
+  </si>
+  <si>
+    <t>Continuer la maquette Haute-Fidélité de l'éditeur de niveau.</t>
+  </si>
+  <si>
+    <t>Commencer la rédaction du rapport.</t>
   </si>
 </sst>
 </file>
@@ -1139,13 +1145,13 @@
                   <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>255</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,16 +1994,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.37634408602150538</c:v>
+                  <c:v>0.31531531531531531</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54838709677419351</c:v>
+                  <c:v>0.54054054054054057</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5268817204301078E-2</c:v>
+                  <c:v>0.14414414414414414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4183,7 +4189,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4238,7 +4244,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>7 heures 45 minutes</v>
+        <v>9 heures 15 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4257,11 +4263,11 @@
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>285</v>
+        <v>375</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>465</v>
+        <v>555</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4668,28 +4674,46 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="str">
+      <c r="A21" s="74">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v/>
-      </c>
-      <c r="B21" s="40"/>
+        <v>39</v>
+      </c>
+      <c r="B21" s="40">
+        <v>45558</v>
+      </c>
       <c r="C21" s="41"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="28"/>
+      <c r="D21" s="42">
+        <v>45</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>52</v>
+      </c>
       <c r="G21" s="46"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="str">
+      <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v/>
-      </c>
-      <c r="B22" s="36"/>
+        <v>4</v>
+      </c>
+      <c r="B22" s="36">
+        <v>23</v>
+      </c>
       <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="45"/>
+      <c r="D22" s="38">
+        <v>45</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="74" t="str">
@@ -10967,7 +10991,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.37634408602150538</v>
+        <v>0.31531531531531531</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -10988,11 +11012,11 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>255</v>
+        <v>300</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11000,11 +11024,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>4 h 15 min</v>
+        <v>5 h 00 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.54838709677419351</v>
+        <v>0.54054054054054057</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11062,11 +11086,11 @@
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11074,11 +11098,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>0 h 35 min</v>
+        <v>1 h 20 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>7.5268817204301078E-2</v>
+        <v>0.14414414414414414</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11099,22 +11123,22 @@
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>285</v>
+        <v>375</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>465</v>
+        <v>555</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>7 h 45 min</v>
+        <v>9 h 15 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>8.8068181818181823E-2</v>
+        <v>0.10511363636363637</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11145,7 +11169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F31118-7D2C-C547-B9C9-EA2B04E048B8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
@@ -11158,26 +11182,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34298955776df91f451dfdd912b0d80d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed9741631eefaa61c396a6d47d02de0f" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11372,28 +11376,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE95A31-3997-42E6-AE6E-094AD61D4048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11410,4 +11413,25 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
chore(UX): jdt, rapport et todolist
</commit_message>
<xml_diff>
--- a/UX/jdt/JDT_OlayaMathis.xlsx
+++ b/UX/jdt/JDT_OlayaMathis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg24muu\Documents\GitHub\P_ShootMeUp\UX\jdt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C02C05-1F53-490E-B52A-AAD8CDCB54FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE89DCB-334C-4EA3-A658-3B9975B9092E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>Auteur:</t>
   </si>
@@ -203,6 +203,15 @@
   </si>
   <si>
     <t>Commencer la rédaction du rapport.</t>
+  </si>
+  <si>
+    <t>Remplir l'auto-évaluation</t>
+  </si>
+  <si>
+    <t>Améliorer la maquette high-fidelity</t>
+  </si>
+  <si>
+    <t>Continuer la rédaction du rapport.</t>
   </si>
 </sst>
 </file>
@@ -1145,13 +1154,13 @@
                   <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>300</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1994,16 +2003,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.31531531531531531</c:v>
+                  <c:v>0.23809523809523808</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54054054054054057</c:v>
+                  <c:v>0.51020408163265307</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14414414414414414</c:v>
+                  <c:v>0.25170068027210885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4189,7 +4198,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4244,7 +4253,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>9 heures 15 minutes</v>
+        <v>12 heures 15 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4259,15 +4268,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>555</v>
+        <v>735</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4696,10 +4705,10 @@
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="73">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="B22" s="36">
-        <v>23</v>
+        <v>45558</v>
       </c>
       <c r="C22" s="37"/>
       <c r="D22" s="38">
@@ -4716,39 +4725,67 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="74" t="str">
+      <c r="A23" s="74">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v/>
-      </c>
-      <c r="B23" s="40"/>
+        <v>41</v>
+      </c>
+      <c r="B23" s="40">
+        <v>45572</v>
+      </c>
       <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="28"/>
+      <c r="D23" s="42">
+        <v>15</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>54</v>
+      </c>
       <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="73" t="str">
+      <c r="A24" s="73">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v/>
-      </c>
-      <c r="B24" s="36"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="28"/>
+        <v>41</v>
+      </c>
+      <c r="B24" s="36">
+        <v>45572</v>
+      </c>
+      <c r="C24" s="37">
+        <v>1</v>
+      </c>
+      <c r="D24" s="38">
+        <v>15</v>
+      </c>
+      <c r="E24" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>55</v>
+      </c>
       <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="74" t="str">
+      <c r="A25" s="74">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v/>
-      </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="28"/>
+        <v>41</v>
+      </c>
+      <c r="B25" s="40">
+        <v>45572</v>
+      </c>
+      <c r="C25" s="41">
+        <v>1</v>
+      </c>
+      <c r="D25" s="42">
+        <v>30</v>
+      </c>
+      <c r="E25" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>56</v>
+      </c>
       <c r="G25" s="46"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -10991,7 +11028,7 @@
       </c>
       <c r="G6" s="47">
         <f>SUM(A6:B6)/$C$10</f>
-        <v>0.31531531531531531</v>
+        <v>0.23809523809523808</v>
       </c>
       <c r="L6" s="62" t="str">
         <f>'Journal de travail'!M8</f>
@@ -11008,15 +11045,15 @@
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>375</v>
       </c>
       <c r="E7" s="30" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11024,11 +11061,11 @@
       </c>
       <c r="F7" s="55" t="str">
         <f t="shared" ref="F7:F10" si="1">QUOTIENT(SUM(A7:B7),60)&amp;" h "&amp;TEXT(MOD(SUM(A7:B7),60), "00")&amp;" min"</f>
-        <v>5 h 00 min</v>
+        <v>6 h 15 min</v>
       </c>
       <c r="G7" s="56">
         <f t="shared" ref="G7:G9" si="2">SUM(A7:B7)/$C$10</f>
-        <v>0.54054054054054057</v>
+        <v>0.51020408163265307</v>
       </c>
       <c r="L7" s="64" t="str">
         <f>'Journal de travail'!M9</f>
@@ -11082,15 +11119,15 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="B9">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Plannification!E9,'Journal de travail'!$D$7:$D$532)</f>
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>185</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11098,11 +11135,11 @@
       </c>
       <c r="F9" s="55" t="str">
         <f t="shared" si="1"/>
-        <v>1 h 20 min</v>
+        <v>3 h 05 min</v>
       </c>
       <c r="G9" s="56">
         <f t="shared" si="2"/>
-        <v>0.14414414414414414</v>
+        <v>0.25170068027210885</v>
       </c>
       <c r="L9" s="66" t="str">
         <f>'Journal de travail'!M11</f>
@@ -11119,26 +11156,26 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>SUM(A6:A9)</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="B10">
         <f>SUM(B6:B9)</f>
-        <v>375</v>
+        <v>435</v>
       </c>
       <c r="C10">
         <f>SUM(A10:B10)</f>
-        <v>555</v>
+        <v>735</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="50" t="str">
         <f t="shared" si="1"/>
-        <v>9 h 15 min</v>
+        <v>12 h 15 min</v>
       </c>
       <c r="G10" s="57">
         <f>C10/C11</f>
-        <v>0.10511363636363637</v>
+        <v>0.13920454545454544</v>
       </c>
       <c r="L10" s="67" t="s">
         <v>18</v>
@@ -11182,6 +11219,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010080C9F2488912074FB587B9AD9ADAE5BB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="34298955776df91f451dfdd912b0d80d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5cf4370-ac38-4b9e-9836-ef6f5df64f24" xmlns:ns3="eefa3612-053e-497a-ae76-8a76877f5e22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ed9741631eefaa61c396a6d47d02de0f" ns2:_="" ns3:_="">
     <xsd:import namespace="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
@@ -11376,27 +11433,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
+    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5cf4370-ac38-4b9e-9836-ef6f5df64f24">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE95A31-3997-42E6-AE6E-094AD61D4048}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11413,25 +11471,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
-    <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>